<commit_message>
Deploy dhhepting/dhhepting.github.io to github.com/dhhepting/dhhepting.github.io.git:gh-pages
</commit_message>
<xml_diff>
--- a/_data/teaching/feedback/CS-428_828-201930-midterm.xlsx
+++ b/_data/teaching/feedback/CS-428_828-201930-midterm.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hepting/Sites/dhhepting.github.io/_data/teaching/feedback/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{CB42672A-6632-2442-8D10-F25B884C11EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43640B78-AB36-2848-93ED-39C6E5FDFA4A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2600" yWindow="1100" windowWidth="25040" windowHeight="16900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3660" yWindow="1980" windowWidth="25040" windowHeight="16900" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="feedback" sheetId="1" r:id="rId1"/>
+    <sheet name="_h2_assigned_courses__h2_ (39)" sheetId="2" r:id="rId1"/>
+    <sheet name="feedback" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
   <si>
     <t>q1</t>
   </si>
@@ -79,6 +80,36 @@
   </si>
   <si>
     <t>median</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>890DW</t>
+  </si>
+  <si>
+    <t>890DE</t>
+  </si>
+  <si>
+    <t>490CN</t>
+  </si>
+  <si>
+    <t>490AB</t>
+  </si>
+  <si>
+    <t>Enrollment</t>
+  </si>
+  <si>
+    <t>Section Number</t>
+  </si>
+  <si>
+    <t>Course Number</t>
+  </si>
+  <si>
+    <t>Subject Code</t>
+  </si>
+  <si>
+    <t>CRN</t>
   </si>
 </sst>
 </file>
@@ -523,11 +554,279 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D53DE6BC-389E-8040-9BBA-04147C39B4A1}">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>10667</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2">
+        <v>205</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>10680</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>280</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>13499</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>13495</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>10705</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6">
+        <v>499</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>10706</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7">
+        <v>499</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>13229</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>13496</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>10716</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10">
+        <v>900</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10717</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11">
+        <v>900</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>10718</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12">
+        <v>900</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>10719</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13">
+        <v>900</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>10723</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14">
+        <v>901</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>10738</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15">
+        <v>902</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="K76" sqref="K76"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4259,11 +4558,11 @@
         <v>4.6266666666666669</v>
       </c>
       <c r="C77" s="1">
-        <f t="shared" ref="C77:J77" si="56">AVERAGE(C2:C76)</f>
+        <f>AVERAGE(C2:C76)</f>
         <v>4.2</v>
       </c>
       <c r="D77" s="1">
-        <f t="shared" si="56"/>
+        <f t="shared" ref="C77:J77" si="56">AVERAGE(D2:D76)</f>
         <v>4.3866666666666667</v>
       </c>
       <c r="E77" s="1">
@@ -4308,7 +4607,7 @@
         <v>0.8944271909999163</v>
       </c>
       <c r="C78" s="1">
-        <f t="shared" si="59"/>
+        <f>STDEV(C2:C6)</f>
         <v>0.83666002653407512</v>
       </c>
       <c r="D78" s="1">

</xml_diff>